<commit_message>
Updated to round 15
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_base_XGB_full.xlsx
+++ b/leagueStats/leagueStats_base_XGB_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O139"/>
+  <dimension ref="A1:O149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7543,6 +7543,516 @@
         <v>2</v>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>2</v>
+      </c>
+      <c r="E140" t="n">
+        <v>1</v>
+      </c>
+      <c r="F140" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="H140" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="I140" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M140" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="N140" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="O140" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>3</v>
+      </c>
+      <c r="E141" t="n">
+        <v>1</v>
+      </c>
+      <c r="F141" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G141" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H141" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="I141" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="J141" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M141" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N141" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="O141" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="G142" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H142" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="I142" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="J142" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M142" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N142" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>2</v>
+      </c>
+      <c r="E143" t="n">
+        <v>2</v>
+      </c>
+      <c r="F143" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="H143" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I143" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="M143" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="N143" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="O143" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>4</v>
+      </c>
+      <c r="E144" t="n">
+        <v>1</v>
+      </c>
+      <c r="F144" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G144" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="H144" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="I144" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="J144" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="n">
+        <v>1</v>
+      </c>
+      <c r="L144" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="M144" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N144" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="O144" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>1</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0</v>
+      </c>
+      <c r="F145" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="G145" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="H145" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I145" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="J145" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="n">
+        <v>1</v>
+      </c>
+      <c r="L145" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M145" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="N145" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="O145" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+      <c r="E146" t="n">
+        <v>4</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="G146" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="H146" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="I146" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="J146" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M146" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N146" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="O146" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G147" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="H147" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I147" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="J147" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M147" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="N147" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="O147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>2</v>
+      </c>
+      <c r="E148" t="n">
+        <v>2</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G148" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="H148" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I148" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="J148" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M148" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="N148" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O148" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>1</v>
+      </c>
+      <c r="E149" t="n">
+        <v>2</v>
+      </c>
+      <c r="F149" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="G149" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="H149" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="I149" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J149" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="M149" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="N149" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="O149" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to round 18
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_base_XGB_full.xlsx
+++ b/leagueStats/leagueStats_base_XGB_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O169"/>
+  <dimension ref="A1:O179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9073,6 +9073,516 @@
         <v>2</v>
       </c>
     </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>0</v>
+      </c>
+      <c r="E170" t="n">
+        <v>3</v>
+      </c>
+      <c r="F170" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="G170" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="H170" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I170" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="J170" t="n">
+        <v>0</v>
+      </c>
+      <c r="K170" t="n">
+        <v>2</v>
+      </c>
+      <c r="L170" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M170" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N170" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="O170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" t="n">
+        <v>2</v>
+      </c>
+      <c r="F171" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="G171" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="H171" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="I171" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="J171" t="n">
+        <v>1</v>
+      </c>
+      <c r="K171" t="n">
+        <v>1</v>
+      </c>
+      <c r="L171" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M171" t="n">
+        <v>0</v>
+      </c>
+      <c r="N171" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="O171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" t="n">
+        <v>1</v>
+      </c>
+      <c r="F172" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G172" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="H172" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="I172" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="J172" t="n">
+        <v>0</v>
+      </c>
+      <c r="K172" t="n">
+        <v>0</v>
+      </c>
+      <c r="L172" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M172" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="N172" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O172" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>2</v>
+      </c>
+      <c r="E173" t="n">
+        <v>1</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="G173" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="H173" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="I173" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="J173" t="n">
+        <v>1</v>
+      </c>
+      <c r="K173" t="n">
+        <v>0</v>
+      </c>
+      <c r="L173" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M173" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="N173" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="O173" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>2</v>
+      </c>
+      <c r="E174" t="n">
+        <v>2</v>
+      </c>
+      <c r="F174" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="G174" t="n">
+        <v>1</v>
+      </c>
+      <c r="H174" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="I174" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="J174" t="n">
+        <v>0</v>
+      </c>
+      <c r="K174" t="n">
+        <v>0</v>
+      </c>
+      <c r="L174" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M174" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N174" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="O174" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>1</v>
+      </c>
+      <c r="E175" t="n">
+        <v>1</v>
+      </c>
+      <c r="F175" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="G175" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="H175" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I175" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="J175" t="n">
+        <v>0</v>
+      </c>
+      <c r="K175" t="n">
+        <v>0</v>
+      </c>
+      <c r="L175" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M175" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N175" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="O175" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>1</v>
+      </c>
+      <c r="E176" t="n">
+        <v>0</v>
+      </c>
+      <c r="F176" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="G176" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="H176" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="I176" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="J176" t="n">
+        <v>1</v>
+      </c>
+      <c r="K176" t="n">
+        <v>0</v>
+      </c>
+      <c r="L176" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="M176" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N176" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="O176" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>2</v>
+      </c>
+      <c r="E177" t="n">
+        <v>2</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="G177" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H177" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="I177" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="J177" t="n">
+        <v>0</v>
+      </c>
+      <c r="K177" t="n">
+        <v>0</v>
+      </c>
+      <c r="L177" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="M177" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="N177" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="O177" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>2</v>
+      </c>
+      <c r="E178" t="n">
+        <v>3</v>
+      </c>
+      <c r="F178" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="G178" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="H178" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="I178" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="J178" t="n">
+        <v>0</v>
+      </c>
+      <c r="K178" t="n">
+        <v>0</v>
+      </c>
+      <c r="L178" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="M178" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="N178" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="O178" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>2</v>
+      </c>
+      <c r="E179" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="G179" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H179" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="I179" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="J179" t="n">
+        <v>1</v>
+      </c>
+      <c r="K179" t="n">
+        <v>0</v>
+      </c>
+      <c r="L179" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M179" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="N179" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="O179" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to round 20
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_base_XGB_full.xlsx
+++ b/leagueStats/leagueStats_base_XGB_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O179"/>
+  <dimension ref="A1:O195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9583,6 +9583,822 @@
         <v>1</v>
       </c>
     </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" t="n">
+        <v>3</v>
+      </c>
+      <c r="F180" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="G180" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="H180" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="I180" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J180" t="n">
+        <v>0</v>
+      </c>
+      <c r="K180" t="n">
+        <v>1</v>
+      </c>
+      <c r="L180" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M180" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="N180" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="O180" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="G181" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="H181" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I181" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="J181" t="n">
+        <v>0</v>
+      </c>
+      <c r="K181" t="n">
+        <v>0</v>
+      </c>
+      <c r="L181" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M181" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N181" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="O181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>1</v>
+      </c>
+      <c r="E182" t="n">
+        <v>1</v>
+      </c>
+      <c r="F182" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G182" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="H182" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I182" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="J182" t="n">
+        <v>0</v>
+      </c>
+      <c r="K182" t="n">
+        <v>0</v>
+      </c>
+      <c r="L182" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M182" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="N182" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="O182" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G183" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H183" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="I183" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="J183" t="n">
+        <v>0</v>
+      </c>
+      <c r="K183" t="n">
+        <v>1</v>
+      </c>
+      <c r="L183" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M183" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="N183" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="O183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" t="n">
+        <v>2</v>
+      </c>
+      <c r="F184" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="G184" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="H184" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="I184" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="J184" t="n">
+        <v>1</v>
+      </c>
+      <c r="K184" t="n">
+        <v>0</v>
+      </c>
+      <c r="L184" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M184" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="N184" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="O184" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>2</v>
+      </c>
+      <c r="E185" t="n">
+        <v>0</v>
+      </c>
+      <c r="F185" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="G185" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="H185" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="I185" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="J185" t="n">
+        <v>0</v>
+      </c>
+      <c r="K185" t="n">
+        <v>0</v>
+      </c>
+      <c r="L185" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="M185" t="n">
+        <v>0</v>
+      </c>
+      <c r="N185" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="O185" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" t="n">
+        <v>0</v>
+      </c>
+      <c r="F186" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="G186" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H186" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="I186" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="J186" t="n">
+        <v>0</v>
+      </c>
+      <c r="K186" t="n">
+        <v>0</v>
+      </c>
+      <c r="L186" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="M186" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N186" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="O186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>1</v>
+      </c>
+      <c r="E187" t="n">
+        <v>1</v>
+      </c>
+      <c r="F187" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="G187" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="H187" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I187" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="J187" t="n">
+        <v>0</v>
+      </c>
+      <c r="K187" t="n">
+        <v>0</v>
+      </c>
+      <c r="L187" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="M187" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="N187" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="O187" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>1</v>
+      </c>
+      <c r="E188" t="n">
+        <v>3</v>
+      </c>
+      <c r="F188" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="G188" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="H188" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I188" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="J188" t="n">
+        <v>0</v>
+      </c>
+      <c r="K188" t="n">
+        <v>0</v>
+      </c>
+      <c r="L188" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M188" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="N188" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="O188" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>1</v>
+      </c>
+      <c r="E189" t="n">
+        <v>1</v>
+      </c>
+      <c r="F189" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="G189" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H189" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="I189" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="J189" t="n">
+        <v>1</v>
+      </c>
+      <c r="K189" t="n">
+        <v>0</v>
+      </c>
+      <c r="L189" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M189" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N189" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>1</v>
+      </c>
+      <c r="E190" t="n">
+        <v>1</v>
+      </c>
+      <c r="F190" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="G190" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H190" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="I190" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="J190" t="n">
+        <v>0</v>
+      </c>
+      <c r="K190" t="n">
+        <v>0</v>
+      </c>
+      <c r="L190" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="M190" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="N190" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O190" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>0</v>
+      </c>
+      <c r="E191" t="n">
+        <v>0</v>
+      </c>
+      <c r="F191" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="G191" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="H191" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I191" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J191" t="n">
+        <v>1</v>
+      </c>
+      <c r="K191" t="n">
+        <v>0</v>
+      </c>
+      <c r="L191" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M191" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N191" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="O191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>2</v>
+      </c>
+      <c r="E192" t="n">
+        <v>2</v>
+      </c>
+      <c r="F192" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="G192" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H192" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="I192" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="J192" t="n">
+        <v>1</v>
+      </c>
+      <c r="K192" t="n">
+        <v>1</v>
+      </c>
+      <c r="L192" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M192" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N192" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="O192" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>1</v>
+      </c>
+      <c r="E193" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="G193" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="H193" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="I193" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J193" t="n">
+        <v>0</v>
+      </c>
+      <c r="K193" t="n">
+        <v>0</v>
+      </c>
+      <c r="L193" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M193" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="N193" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>2</v>
+      </c>
+      <c r="E194" t="n">
+        <v>0</v>
+      </c>
+      <c r="F194" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="G194" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="H194" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="I194" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="J194" t="n">
+        <v>0</v>
+      </c>
+      <c r="K194" t="n">
+        <v>0</v>
+      </c>
+      <c r="L194" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="M194" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N194" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O194" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>0</v>
+      </c>
+      <c r="E195" t="n">
+        <v>1</v>
+      </c>
+      <c r="F195" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="G195" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="H195" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="I195" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="J195" t="n">
+        <v>0</v>
+      </c>
+      <c r="K195" t="n">
+        <v>0</v>
+      </c>
+      <c r="L195" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M195" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N195" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="O195" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded to Round 20
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_base_XGB_full.xlsx
+++ b/leagueStats/leagueStats_base_XGB_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O195"/>
+  <dimension ref="A1:O199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10399,6 +10399,210 @@
         <v>1</v>
       </c>
     </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>2</v>
+      </c>
+      <c r="E196" t="n">
+        <v>1</v>
+      </c>
+      <c r="F196" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G196" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="H196" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I196" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="J196" t="n">
+        <v>0</v>
+      </c>
+      <c r="K196" t="n">
+        <v>1</v>
+      </c>
+      <c r="L196" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="M196" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="N196" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O196" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>1</v>
+      </c>
+      <c r="E197" t="n">
+        <v>1</v>
+      </c>
+      <c r="F197" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="G197" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="H197" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="I197" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="J197" t="n">
+        <v>0</v>
+      </c>
+      <c r="K197" t="n">
+        <v>0</v>
+      </c>
+      <c r="L197" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="M197" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="N197" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="O197" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>1</v>
+      </c>
+      <c r="E198" t="n">
+        <v>2</v>
+      </c>
+      <c r="F198" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="G198" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="H198" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="I198" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="J198" t="n">
+        <v>0</v>
+      </c>
+      <c r="K198" t="n">
+        <v>0</v>
+      </c>
+      <c r="L198" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M198" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="N198" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O198" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>2</v>
+      </c>
+      <c r="E199" t="n">
+        <v>2</v>
+      </c>
+      <c r="F199" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="G199" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="H199" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="I199" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="J199" t="n">
+        <v>1</v>
+      </c>
+      <c r="K199" t="n">
+        <v>0</v>
+      </c>
+      <c r="L199" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M199" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N199" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="O199" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to Round 25
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_base_XGB_full.xlsx
+++ b/leagueStats/leagueStats_base_XGB_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O130"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7084,6 +7084,465 @@
         <v>2</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H131" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="J131" t="n">
+        <v>1</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>3</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="H132" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="J132" t="n">
+        <v>2</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="O132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
+      <c r="F133" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="G133" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="H133" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="I133" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="n">
+        <v>1</v>
+      </c>
+      <c r="L133" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="M133" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="N133" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="O133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>3</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H134" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="I134" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0</v>
+      </c>
+      <c r="L134" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M134" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="N134" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="O134" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+      <c r="F135" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="G135" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H135" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="I135" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="J135" t="n">
+        <v>1</v>
+      </c>
+      <c r="K135" t="n">
+        <v>1</v>
+      </c>
+      <c r="L135" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M135" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="N135" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="O135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>3</v>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="G136" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H136" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="I136" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="n">
+        <v>1</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="N136" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="O136" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G137" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="H137" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I137" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M137" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="N137" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="O137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="n">
+        <v>2</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G138" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="H138" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I138" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="J138" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="n">
+        <v>1</v>
+      </c>
+      <c r="L138" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M138" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="N138" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>2</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G139" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H139" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I139" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="O139" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>